<commit_message>
Nombres en los headers de 4, 7, 8 y 11
</commit_message>
<xml_diff>
--- a/speedup.xlsx
+++ b/speedup.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\workspace\multiprocessors\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\workspace\team-multi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDA99982-6F5F-483D-AE39-615A6416D38A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2EB450B-EB3F-4201-AB4D-61F1E806AEE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="28">
   <si>
     <t>C</t>
   </si>
@@ -106,6 +106,18 @@
   </si>
   <si>
     <t>31248.98840 ms</t>
+  </si>
+  <si>
+    <t>10.60790 ms</t>
+  </si>
+  <si>
+    <t>215.2952 ms</t>
+  </si>
+  <si>
+    <t>0.8116 ms</t>
+  </si>
+  <si>
+    <t>29615.0306 ms</t>
   </si>
 </sst>
 </file>
@@ -453,8 +465,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -656,6 +668,9 @@
       <c r="B13" t="s">
         <v>19</v>
       </c>
+      <c r="D13" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14">
@@ -844,8 +859,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90475D11-3029-4BDA-9B2E-88D650C89218}">
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -950,7 +965,9 @@
       <c r="C6" s="2">
         <v>2843.8640999999998</v>
       </c>
-      <c r="D6" s="2"/>
+      <c r="D6" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -994,7 +1011,9 @@
         <v>16</v>
       </c>
       <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
+      <c r="D9" s="2" t="s">
+        <v>26</v>
+      </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -1009,7 +1028,9 @@
         <v>12</v>
       </c>
       <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
+      <c r="D10" s="2" t="s">
+        <v>27</v>
+      </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
@@ -1038,6 +1059,9 @@
       </c>
       <c r="B13" t="s">
         <v>19</v>
+      </c>
+      <c r="D13" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
4 de threads avanzado
</commit_message>
<xml_diff>
--- a/speedup.xlsx
+++ b/speedup.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\workspace\team-multi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2EB450B-EB3F-4201-AB4D-61F1E806AEE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92B0C9E5-86C3-4A4B-98B1-918907CD1F61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1620" yWindow="1332" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="32">
   <si>
     <t>C</t>
   </si>
@@ -118,6 +118,18 @@
   </si>
   <si>
     <t>29615.0306 ms</t>
+  </si>
+  <si>
+    <t>43.40 ms</t>
+  </si>
+  <si>
+    <t>11289.5 ms</t>
+  </si>
+  <si>
+    <t>222.09420 ms</t>
+  </si>
+  <si>
+    <t>119.40000 ms</t>
   </si>
 </sst>
 </file>
@@ -915,7 +927,9 @@
         <v>4095.3397</v>
       </c>
       <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
+      <c r="E3" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
@@ -962,13 +976,15 @@
       <c r="B6" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="2">
-        <v>2843.8640999999998</v>
+      <c r="C6" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="2"/>
+      <c r="E6" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
@@ -1031,7 +1047,9 @@
       <c r="D10" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E10" s="2"/>
+      <c r="E10" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>

</xml_diff>

<commit_message>
Cambios del profe añadidos fork-join
</commit_message>
<xml_diff>
--- a/speedup.xlsx
+++ b/speedup.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\workspace\team-multi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92B0C9E5-86C3-4A4B-98B1-918907CD1F61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16B3A043-B0CE-41F8-946F-B483C9FC2031}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1620" yWindow="1332" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -871,8 +871,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90475D11-3029-4BDA-9B2E-88D650C89218}">
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1050,7 +1050,9 @@
       <c r="E10" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F10" s="2"/>
+      <c r="F10" s="2">
+        <v>4128.7</v>
+      </c>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>

</xml_diff>

<commit_message>
speedups y nombres agregados tbb
</commit_message>
<xml_diff>
--- a/speedup.xlsx
+++ b/speedup.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\workspace\team-multi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78F9F943-81FB-487C-B846-FB8863876DD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F388A80-D9EC-4FC5-BB77-D899607F99F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="31">
   <si>
     <t>C</t>
   </si>
@@ -124,9 +125,6 @@
   </si>
   <si>
     <t>11289.5 ms</t>
-  </si>
-  <si>
-    <t>222.09420 ms</t>
   </si>
   <si>
     <t>119.40000 ms</t>
@@ -871,8 +869,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90475D11-3029-4BDA-9B2E-88D650C89218}">
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -976,14 +974,14 @@
       <c r="B6" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>30</v>
+      <c r="C6" s="2">
+        <v>222.0942</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>25</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F6" s="2">
         <v>193.2</v>
@@ -1030,7 +1028,9 @@
       <c r="B9" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="2"/>
+      <c r="C9" s="2">
+        <v>278.08589999999998</v>
+      </c>
       <c r="D9" s="2" t="s">
         <v>26</v>
       </c>
@@ -1094,14 +1094,23 @@
       <c r="B13" t="s">
         <v>19</v>
       </c>
-      <c r="D13" t="s">
-        <v>24</v>
+      <c r="C13">
+        <v>10.607900000000001</v>
+      </c>
+      <c r="D13">
+        <v>10.607900000000001</v>
       </c>
       <c r="F13">
         <v>4.9000000000000004</v>
       </c>
       <c r="G13">
         <v>7.4</v>
+      </c>
+      <c r="H13">
+        <v>5.7026000000000003</v>
+      </c>
+      <c r="I13">
+        <v>3.0617999999999999</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
@@ -1186,8 +1195,8 @@
       <c r="F20" s="4"/>
       <c r="G20" s="3"/>
       <c r="H20" s="2">
-        <f>F6/G6</f>
-        <v>0.74422187981510002</v>
+        <f>C6/H6</f>
+        <v>4.8716085940841642</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
@@ -1224,8 +1233,8 @@
       <c r="F23" s="2"/>
       <c r="G23" s="4"/>
       <c r="H23" s="2">
-        <f>F9/G9</f>
-        <v>0</v>
+        <f>C9/H9</f>
+        <v>4.4559406741774676</v>
       </c>
       <c r="I23" s="4"/>
     </row>
@@ -1241,8 +1250,8 @@
       </c>
       <c r="G24" s="2"/>
       <c r="H24" s="2">
-        <f>F10/G10</f>
-        <v>1.1009573078051251</v>
+        <f>C10/H10</f>
+        <v>4.0665558129336228</v>
       </c>
       <c r="I24" s="3"/>
     </row>
@@ -1270,8 +1279,8 @@
         <v>19</v>
       </c>
       <c r="H27">
-        <f>F13/G13</f>
-        <v>0.66216216216216217</v>
+        <f>C13/H13</f>
+        <v>1.8601865815592888</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Archivos de CUDA añadidos
</commit_message>
<xml_diff>
--- a/speedup.xlsx
+++ b/speedup.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\workspace\team-multi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F388A80-D9EC-4FC5-BB77-D899607F99F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22D3B221-F1E7-4687-8A49-D32A2C74D1F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="28">
   <si>
     <t>C</t>
   </si>
@@ -110,15 +110,6 @@
   </si>
   <si>
     <t>10.60790 ms</t>
-  </si>
-  <si>
-    <t>215.2952 ms</t>
-  </si>
-  <si>
-    <t>0.8116 ms</t>
-  </si>
-  <si>
-    <t>29615.0306 ms</t>
   </si>
   <si>
     <t>43.40 ms</t>
@@ -869,8 +860,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90475D11-3029-4BDA-9B2E-88D650C89218}">
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -926,7 +917,7 @@
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
@@ -977,11 +968,11 @@
       <c r="C6" s="2">
         <v>222.0942</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>25</v>
+      <c r="D6" s="2">
+        <v>215.29519999999999</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F6" s="2">
         <v>193.2</v>
@@ -991,6 +982,9 @@
       </c>
       <c r="H6">
         <v>45.589500000000001</v>
+      </c>
+      <c r="I6">
+        <v>73.250900000000001</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
@@ -1031,8 +1025,8 @@
       <c r="C9" s="2">
         <v>278.08589999999998</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>26</v>
+      <c r="D9" s="2">
+        <v>0.81159999999999999</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
@@ -1042,7 +1036,9 @@
       <c r="H9">
         <v>62.407899999999998</v>
       </c>
-      <c r="I9" s="2"/>
+      <c r="I9" s="2">
+        <v>6.6848999999999998</v>
+      </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10">
@@ -1054,11 +1050,11 @@
       <c r="C10" s="2">
         <v>289.3143</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>27</v>
+      <c r="D10" s="2">
+        <v>29615.030599999998</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F10" s="2">
         <v>4128.7</v>
@@ -1069,7 +1065,9 @@
       <c r="H10">
         <v>71.144800000000004</v>
       </c>
-      <c r="I10" s="2"/>
+      <c r="I10" s="2">
+        <v>10041.270399999999</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11">
@@ -1198,6 +1196,10 @@
         <f>C6/H6</f>
         <v>4.8716085940841642</v>
       </c>
+      <c r="I20">
+        <f>D6/I6</f>
+        <v>2.939147505354883</v>
+      </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21">
@@ -1236,7 +1238,10 @@
         <f>C9/H9</f>
         <v>4.4559406741774676</v>
       </c>
-      <c r="I23" s="4"/>
+      <c r="I23" s="4">
+        <f>D9/I9</f>
+        <v>0.12140794925877725</v>
+      </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24">
@@ -1253,7 +1258,10 @@
         <f>C10/H10</f>
         <v>4.0665558129336228</v>
       </c>
-      <c r="I24" s="3"/>
+      <c r="I24" s="3">
+        <f>D10/I10</f>
+        <v>2.9493310527719681</v>
+      </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25">
@@ -1281,6 +1289,10 @@
       <c r="H27">
         <f>C13/H13</f>
         <v>1.8601865815592888</v>
+      </c>
+      <c r="I27">
+        <f>D13/I13</f>
+        <v>3.4645959892873477</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
7 terminado sin probar
</commit_message>
<xml_diff>
--- a/speedup.xlsx
+++ b/speedup.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\workspace\team-multi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22D3B221-F1E7-4687-8A49-D32A2C74D1F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{669E94E6-6FE2-4E40-8012-BE18183E76A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="29">
   <si>
     <t>C</t>
   </si>
@@ -119,12 +118,18 @@
   </si>
   <si>
     <t>119.40000 ms</t>
+  </si>
+  <si>
+    <t>C server</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="0.00000"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -171,7 +176,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1" shrinkToFit="1"/>
@@ -184,6 +189,7 @@
       <alignment horizontal="center" wrapText="1" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -858,54 +864,58 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90475D11-3029-4BDA-9B2E-88D650C89218}">
-  <dimension ref="A1:J29"/>
+  <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="10" width="14.33203125" customWidth="1"/>
+    <col min="3" max="11" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B1" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C1" s="5">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D1" s="5"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -916,15 +926,16 @@
         <v>4095.3397</v>
       </c>
       <c r="D3" s="2"/>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="2"/>
+      <c r="F3" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="F3" s="2"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J3" s="2"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -940,8 +951,9 @@
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J4" s="2"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -957,8 +969,9 @@
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J5" s="2"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -969,25 +982,31 @@
         <v>222.0942</v>
       </c>
       <c r="D6" s="2">
+        <v>166.84059999999999</v>
+      </c>
+      <c r="E6" s="2">
         <v>215.29519999999999</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="F6" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F6" s="2">
+      <c r="G6" s="2">
         <v>193.2</v>
       </c>
-      <c r="G6" s="2">
+      <c r="H6" s="2">
         <v>259.60000000000002</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>45.589500000000001</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>73.250900000000001</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K6" s="8">
+        <v>6.3E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -999,9 +1018,10 @@
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
-      <c r="I7" s="2"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H7" s="2"/>
+      <c r="J7" s="2"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1013,9 +1033,10 @@
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
-      <c r="I8" s="2"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H8" s="2"/>
+      <c r="J8" s="2"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1025,22 +1046,23 @@
       <c r="C9" s="2">
         <v>278.08589999999998</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="2"/>
+      <c r="E9" s="2">
         <v>0.81159999999999999</v>
       </c>
-      <c r="E9" s="2"/>
       <c r="F9" s="2"/>
-      <c r="G9" s="4">
+      <c r="G9" s="2"/>
+      <c r="H9" s="4">
         <v>401.2</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <v>62.407899999999998</v>
       </c>
-      <c r="I9" s="2">
+      <c r="J9" s="2">
         <v>6.6848999999999998</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1050,26 +1072,27 @@
       <c r="C10" s="2">
         <v>289.3143</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="2"/>
+      <c r="E10" s="2">
         <v>29615.030599999998</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="F10" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F10" s="2">
+      <c r="G10" s="2">
         <v>4128.7</v>
       </c>
-      <c r="G10" s="2">
+      <c r="H10" s="2">
         <v>3750.1</v>
       </c>
-      <c r="H10">
+      <c r="I10">
         <v>71.144800000000004</v>
       </c>
-      <c r="I10" s="2">
+      <c r="J10" s="2">
         <v>10041.270399999999</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1077,7 +1100,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1085,7 +1108,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1095,23 +1118,23 @@
       <c r="C13">
         <v>10.607900000000001</v>
       </c>
-      <c r="D13">
+      <c r="E13">
         <v>10.607900000000001</v>
       </c>
-      <c r="F13">
+      <c r="G13">
         <v>4.9000000000000004</v>
       </c>
-      <c r="G13">
+      <c r="H13">
         <v>7.4</v>
       </c>
-      <c r="H13">
+      <c r="I13">
         <v>5.7026000000000003</v>
       </c>
-      <c r="I13">
+      <c r="J13">
         <v>3.0617999999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1119,7 +1142,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>13</v>
       </c>
@@ -1127,143 +1150,148 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B16" s="5"/>
       <c r="C16" s="7"/>
-      <c r="D16" s="5"/>
+      <c r="D16" s="7"/>
       <c r="E16" s="5"/>
-      <c r="F16" s="6" t="s">
+      <c r="F16" s="5"/>
+      <c r="G16" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="G16" s="6" t="s">
+      <c r="H16" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="H16" s="6" t="s">
+      <c r="I16" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="I16" s="6" t="s">
+      <c r="J16" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="J16" s="6" t="s">
+      <c r="K16" s="6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>1</v>
       </c>
       <c r="B17" t="s">
         <v>9</v>
       </c>
-      <c r="F17" s="4"/>
       <c r="G17" s="4"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="2"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H17" s="4"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="2"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>2</v>
       </c>
       <c r="B18" t="s">
         <v>10</v>
       </c>
-      <c r="F18" s="3"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="2"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G18" s="3"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="2"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>3</v>
       </c>
       <c r="B19" t="s">
         <v>13</v>
       </c>
-      <c r="F19" s="2"/>
-      <c r="G19" s="3"/>
-      <c r="I19" s="2"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G19" s="2"/>
+      <c r="H19" s="3"/>
+      <c r="J19" s="2"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>4</v>
       </c>
       <c r="B20" t="s">
         <v>14</v>
       </c>
-      <c r="F20" s="4"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="2">
-        <f>C6/H6</f>
+      <c r="G20" s="4"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="2">
+        <f>C6/I6</f>
         <v>4.8716085940841642</v>
       </c>
-      <c r="I20">
-        <f>D6/I6</f>
+      <c r="J20">
+        <f>E6/J6</f>
         <v>2.939147505354883</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K20">
+        <f>D6/K6</f>
+        <v>26482.634920634919</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>5</v>
       </c>
       <c r="B21" t="s">
         <v>15</v>
       </c>
-      <c r="F21" s="4"/>
       <c r="G21" s="4"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="3"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H21" s="4"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="3"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>6</v>
       </c>
       <c r="B22" t="s">
         <v>11</v>
       </c>
-      <c r="F22" s="2"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="2"/>
-      <c r="I22" s="3"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G22" s="2"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="3"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>7</v>
       </c>
       <c r="B23" t="s">
         <v>16</v>
       </c>
-      <c r="F23" s="2"/>
-      <c r="G23" s="4"/>
-      <c r="H23" s="2">
-        <f>C9/H9</f>
+      <c r="G23" s="2"/>
+      <c r="H23" s="4"/>
+      <c r="I23" s="2">
+        <f>C9/I9</f>
         <v>4.4559406741774676</v>
       </c>
-      <c r="I23" s="4">
-        <f>D9/I9</f>
+      <c r="J23" s="4">
+        <f>E9/J9</f>
         <v>0.12140794925877725</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>8</v>
       </c>
       <c r="B24" t="s">
         <v>12</v>
       </c>
-      <c r="F24" s="4">
+      <c r="G24" s="4">
         <v>4529.6000000000004</v>
       </c>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2">
-        <f>C10/H10</f>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2">
+        <f>C10/I10</f>
         <v>4.0665558129336228</v>
       </c>
-      <c r="I24" s="3">
-        <f>D10/I10</f>
+      <c r="J24" s="3">
+        <f>E10/J10</f>
         <v>2.9493310527719681</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>9</v>
       </c>
@@ -1271,7 +1299,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>10</v>
       </c>
@@ -1279,23 +1307,23 @@
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>11</v>
       </c>
       <c r="B27" t="s">
         <v>19</v>
       </c>
-      <c r="H27">
-        <f>C13/H13</f>
+      <c r="I27">
+        <f>C13/I13</f>
         <v>1.8601865815592888</v>
       </c>
-      <c r="I27">
-        <f>D13/I13</f>
+      <c r="J27">
+        <f>E13/J13</f>
         <v>3.4645959892873477</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>12</v>
       </c>
@@ -1303,7 +1331,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>13</v>
       </c>

</xml_diff>

<commit_message>
cambios en el 8
</commit_message>
<xml_diff>
--- a/speedup.xlsx
+++ b/speedup.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\workspace\team-multi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{669E94E6-6FE2-4E40-8012-BE18183E76A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C95D9C7-BC07-43DD-9210-7AD63E817CED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -866,8 +866,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90475D11-3029-4BDA-9B2E-88D650C89218}">
   <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1046,7 +1046,9 @@
       <c r="C9" s="2">
         <v>278.08589999999998</v>
       </c>
-      <c r="D9" s="2"/>
+      <c r="D9" s="2">
+        <v>168.0162</v>
+      </c>
       <c r="E9" s="2">
         <v>0.81159999999999999</v>
       </c>
@@ -1060,6 +1062,9 @@
       </c>
       <c r="J9" s="2">
         <v>6.6848999999999998</v>
+      </c>
+      <c r="K9" s="8">
+        <v>5.7000000000000002E-3</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
@@ -1270,6 +1275,10 @@
         <f>E9/J9</f>
         <v>0.12140794925877725</v>
       </c>
+      <c r="K23">
+        <f>D9/K9</f>
+        <v>29476.526315789473</v>
+      </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24">

</xml_diff>

<commit_message>
Comentarios de speedup agregados a cuda
</commit_message>
<xml_diff>
--- a/speedup.xlsx
+++ b/speedup.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\workspace\team-multi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C95D9C7-BC07-43DD-9210-7AD63E817CED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CAEEE12-AE64-4937-8DFE-1E033D475A07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -156,12 +156,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -176,7 +188,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1" shrinkToFit="1"/>
@@ -189,7 +201,12 @@
       <alignment horizontal="center" wrapText="1" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -866,8 +883,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90475D11-3029-4BDA-9B2E-88D650C89218}">
   <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1002,7 +1019,7 @@
       <c r="J6">
         <v>73.250900000000001</v>
       </c>
-      <c r="K6" s="8">
+      <c r="K6" s="10">
         <v>6.3E-3</v>
       </c>
     </row>
@@ -1063,7 +1080,7 @@
       <c r="J9" s="2">
         <v>6.6848999999999998</v>
       </c>
-      <c r="K9" s="8">
+      <c r="K9" s="10">
         <v>5.7000000000000002E-3</v>
       </c>
     </row>
@@ -1077,7 +1094,9 @@
       <c r="C10" s="2">
         <v>289.3143</v>
       </c>
-      <c r="D10" s="2"/>
+      <c r="D10" s="2">
+        <v>215.2542</v>
+      </c>
       <c r="E10" s="2">
         <v>29615.030599999998</v>
       </c>
@@ -1095,6 +1114,9 @@
       </c>
       <c r="J10" s="2">
         <v>10041.270399999999</v>
+      </c>
+      <c r="K10" s="11">
+        <v>3.8999999999999998E-3</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
@@ -1173,7 +1195,7 @@
       <c r="J16" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="K16" s="6" t="s">
+      <c r="K16" s="9" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1229,7 +1251,7 @@
         <f>E6/J6</f>
         <v>2.939147505354883</v>
       </c>
-      <c r="K20">
+      <c r="K20" s="8">
         <f>D6/K6</f>
         <v>26482.634920634919</v>
       </c>
@@ -1275,7 +1297,7 @@
         <f>E9/J9</f>
         <v>0.12140794925877725</v>
       </c>
-      <c r="K23">
+      <c r="K23" s="8">
         <f>D9/K9</f>
         <v>29476.526315789473</v>
       </c>
@@ -1298,6 +1320,10 @@
       <c r="J24" s="3">
         <f>E10/J10</f>
         <v>2.9493310527719681</v>
+      </c>
+      <c r="K24" s="8">
+        <f>D10/K10</f>
+        <v>55193.384615384617</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">

</xml_diff>